<commit_message>
Move File Activity added
</commit_message>
<xml_diff>
--- a/ScrapedInvoiceOutput.xlsx
+++ b/ScrapedInvoiceOutput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aykut\Documents\UiPath\Bot5_PDFDataScrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DC9CEA-75F1-496F-B43A-13C81A144078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DF983C-5655-4A8C-BB45-EAFB06E00F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="2115" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-4305" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -82,10 +82,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +400,7 @@
   <dimension ref="A1:G173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,6 +411,7 @@
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="69.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -431,7 +441,13 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>

</xml_diff>